<commit_message>
update with NE and NW traverses
</commit_message>
<xml_diff>
--- a/planning_info/S_chartering_2021_Nordland.xlsx
+++ b/planning_info/S_chartering_2021_Nordland.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="105">
   <si>
     <t>date (YYYY-MM-DD)</t>
   </si>
@@ -106,9 +106,6 @@
     <t>2021-06-25</t>
   </si>
   <si>
-    <t>2021-08-01</t>
-  </si>
-  <si>
     <t>Wednesday</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>NSE</t>
   </si>
   <si>
-    <t>SWC</t>
-  </si>
-  <si>
     <t>473</t>
   </si>
   <si>
@@ -241,9 +235,6 @@
     <t>142</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>end of flying</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t>0.6</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>Akureyri</t>
   </si>
   <si>
@@ -292,9 +280,6 @@
     <t>NASA-SE</t>
   </si>
   <si>
-    <t>Swiss Camp</t>
-  </si>
-  <si>
     <t>transit to Greenland. bring any cargo from Iceland?</t>
   </si>
   <si>
@@ -344,9 +329,6 @@
   </si>
   <si>
     <t>transit to AEY</t>
-  </si>
-  <si>
-    <t>return empty to JAV</t>
   </si>
 </sst>
 </file>
@@ -704,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -777,19 +759,19 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2">
         <v>8.5</v>
       </c>
       <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
         <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -798,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J2">
         <v>3.8</v>
@@ -807,7 +789,7 @@
         <v>12.3</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2">
         <v>65.65470000000001</v>
@@ -822,16 +804,16 @@
         <v>-37.1349</v>
       </c>
       <c r="Q2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="R2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S2">
         <v>140</v>
       </c>
       <c r="T2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -839,19 +821,19 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3">
         <v>8.5</v>
       </c>
       <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
         <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -860,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J3">
         <v>3.1</v>
@@ -869,7 +851,7 @@
         <v>16.4</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M3">
         <v>65.5745</v>
@@ -884,21 +866,21 @@
         <v>-51.6742</v>
       </c>
       <c r="Q3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="R3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S3">
         <v>140</v>
       </c>
       <c r="T3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="I4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J4">
         <v>6.1</v>
@@ -909,13 +891,13 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -923,19 +905,19 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>8.25</v>
       </c>
       <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
         <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
       </c>
       <c r="G6">
         <v>750</v>
@@ -944,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J6">
         <v>1.6</v>
@@ -953,7 +935,7 @@
         <v>9.9</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6">
         <v>64.1917</v>
@@ -968,16 +950,16 @@
         <v>-50.711</v>
       </c>
       <c r="Q6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="R6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S6">
         <v>140</v>
       </c>
       <c r="T6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -985,28 +967,28 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>8.25</v>
       </c>
       <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="F7" t="s">
-        <v>52</v>
-      </c>
       <c r="G7">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H7">
         <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J7">
         <v>1.2</v>
@@ -1015,7 +997,7 @@
         <v>12.1</v>
       </c>
       <c r="L7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M7">
         <v>67.0106</v>
@@ -1030,16 +1012,16 @@
         <v>-46.2789</v>
       </c>
       <c r="Q7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="R7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="S7">
         <v>140</v>
       </c>
       <c r="T7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1047,28 +1029,28 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>8.25</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J8">
         <v>1.2</v>
@@ -1077,7 +1059,7 @@
         <v>17.7</v>
       </c>
       <c r="L8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M8">
         <v>66.48</v>
@@ -1092,21 +1074,21 @@
         <v>-50.711</v>
       </c>
       <c r="Q8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="R8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S8">
         <v>140</v>
       </c>
       <c r="T8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="I9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J9">
         <v>2.8</v>
@@ -1117,28 +1099,28 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>8.5</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H10">
         <v>3</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J10">
         <v>1.6</v>
@@ -1147,7 +1129,7 @@
         <v>10.1</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="M10">
         <v>67.0106</v>
@@ -1162,16 +1144,16 @@
         <v>-44.5002</v>
       </c>
       <c r="Q10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="R10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="S10">
         <v>140</v>
       </c>
       <c r="T10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1179,28 +1161,28 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>8.5</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J11">
         <v>0.8</v>
@@ -1209,7 +1191,7 @@
         <v>11.5</v>
       </c>
       <c r="L11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M11">
         <v>65.9995</v>
@@ -1224,16 +1206,16 @@
         <v>-46.2789</v>
       </c>
       <c r="Q11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="R11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="S11">
         <v>140</v>
       </c>
       <c r="T11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1241,28 +1223,28 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>8.5</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J12">
         <v>1.2</v>
@@ -1271,7 +1253,7 @@
         <v>17.2</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M12">
         <v>66.48</v>
@@ -1286,21 +1268,21 @@
         <v>-50.711</v>
       </c>
       <c r="Q12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="R12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S12">
         <v>140</v>
       </c>
       <c r="T12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="I13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J13">
         <v>2.3</v>
@@ -1311,28 +1293,28 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>8.5</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="H14">
         <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J14">
         <v>1.8</v>
@@ -1341,7 +1323,7 @@
         <v>10.3</v>
       </c>
       <c r="L14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M14">
         <v>67.0106</v>
@@ -1356,16 +1338,16 @@
         <v>-46.9867</v>
       </c>
       <c r="Q14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="R14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="S14">
         <v>140</v>
       </c>
       <c r="T14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1373,28 +1355,28 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>8.5</v>
       </c>
       <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
         <v>54</v>
       </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
       <c r="G15">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="H15">
         <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J15">
         <v>1.1</v>
@@ -1403,7 +1385,7 @@
         <v>15.8</v>
       </c>
       <c r="L15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M15">
         <v>69.8798</v>
@@ -1418,21 +1400,21 @@
         <v>-51.0664</v>
       </c>
       <c r="Q15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="R15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="S15">
         <v>140</v>
       </c>
       <c r="T15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="I16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J16">
         <v>2</v>
@@ -1443,13 +1425,13 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -1457,28 +1439,28 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18">
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H18">
         <v>3</v>
       </c>
       <c r="I18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J18">
         <v>1.8</v>
@@ -1487,7 +1469,7 @@
         <v>9.800000000000001</v>
       </c>
       <c r="L18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M18">
         <v>69.2405</v>
@@ -1502,16 +1484,16 @@
         <v>-46.2789</v>
       </c>
       <c r="Q18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="S18">
         <v>140</v>
       </c>
       <c r="T18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -1519,28 +1501,28 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19">
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H19">
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J19">
         <v>1.9</v>
@@ -1549,7 +1531,7 @@
         <v>12.3</v>
       </c>
       <c r="L19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M19">
         <v>66.48</v>
@@ -1564,16 +1546,16 @@
         <v>-44.8172</v>
       </c>
       <c r="Q19" t="s">
+        <v>81</v>
+      </c>
+      <c r="R19" t="s">
         <v>85</v>
-      </c>
-      <c r="R19" t="s">
-        <v>89</v>
       </c>
       <c r="S19">
         <v>140</v>
       </c>
       <c r="T19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -1581,28 +1563,28 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>8</v>
       </c>
       <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" t="s">
         <v>56</v>
       </c>
-      <c r="F20" t="s">
-        <v>57</v>
-      </c>
       <c r="G20">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H20">
         <v>3</v>
       </c>
       <c r="I20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J20">
         <v>1.3</v>
@@ -1611,7 +1593,7 @@
         <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M20">
         <v>63.1489</v>
@@ -1626,21 +1608,21 @@
         <v>-45.4178</v>
       </c>
       <c r="Q20" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="R20" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="S20">
         <v>140</v>
       </c>
       <c r="T20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="I21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J21">
         <v>3.7</v>
@@ -1651,28 +1633,28 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H22">
         <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J22">
         <v>2.2</v>
@@ -1681,7 +1663,7 @@
         <v>10.2</v>
       </c>
       <c r="L22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M22">
         <v>61.1614</v>
@@ -1696,21 +1678,21 @@
         <v>-51.6742</v>
       </c>
       <c r="Q22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="R22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S22">
         <v>140</v>
       </c>
       <c r="T22" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:20">
       <c r="I23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J23">
         <v>1.8</v>
@@ -1721,28 +1703,28 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24">
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G24">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H24">
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J24">
         <v>2.3</v>
@@ -1751,7 +1733,7 @@
         <v>10.3</v>
       </c>
       <c r="L24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M24">
         <v>64.1917</v>
@@ -1766,16 +1748,16 @@
         <v>-42.5002</v>
       </c>
       <c r="Q24" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="R24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="S24">
         <v>140</v>
       </c>
       <c r="T24" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -1783,28 +1765,28 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G25">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H25">
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J25">
         <v>1.4</v>
@@ -1813,7 +1795,7 @@
         <v>16.2</v>
       </c>
       <c r="L25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M25">
         <v>66.47969999999999</v>
@@ -1828,21 +1810,21 @@
         <v>-37.1349</v>
       </c>
       <c r="Q25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="R25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S25">
         <v>140</v>
       </c>
       <c r="T25" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:20">
       <c r="I26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J26">
         <v>2.9</v>
@@ -1853,28 +1835,28 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G27">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H27">
         <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J27">
         <v>3.8</v>
@@ -1883,7 +1865,7 @@
         <v>11.8</v>
       </c>
       <c r="L27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M27">
         <v>65.5745</v>
@@ -1898,156 +1880,24 @@
         <v>-18.0757</v>
       </c>
       <c r="Q27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="R27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="S27">
         <v>140</v>
       </c>
       <c r="T27" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:20">
       <c r="I28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J28">
         <v>3.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29">
-        <v>8.5</v>
-      </c>
-      <c r="E29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29">
-        <v>150</v>
-      </c>
-      <c r="H29">
-        <v>4</v>
-      </c>
-      <c r="I29" t="s">
-        <v>75</v>
-      </c>
-      <c r="J29">
-        <v>0.7</v>
-      </c>
-      <c r="K29">
-        <v>9.199999999999999</v>
-      </c>
-      <c r="L29" t="s">
-        <v>80</v>
-      </c>
-      <c r="M29">
-        <v>69.2405</v>
-      </c>
-      <c r="N29">
-        <v>-51.0664</v>
-      </c>
-      <c r="O29">
-        <v>69.56829999999999</v>
-      </c>
-      <c r="P29">
-        <v>-49.3158</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>88</v>
-      </c>
-      <c r="R29" t="s">
-        <v>92</v>
-      </c>
-      <c r="S29">
-        <v>140</v>
-      </c>
-      <c r="T29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30">
-        <v>8.5</v>
-      </c>
-      <c r="E30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" t="s">
-        <v>55</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>4</v>
-      </c>
-      <c r="I30" t="s">
-        <v>75</v>
-      </c>
-      <c r="J30">
-        <v>0.7</v>
-      </c>
-      <c r="K30">
-        <v>10.4</v>
-      </c>
-      <c r="L30" t="s">
-        <v>80</v>
-      </c>
-      <c r="M30">
-        <v>69.56829999999999</v>
-      </c>
-      <c r="N30">
-        <v>-49.3158</v>
-      </c>
-      <c r="O30">
-        <v>69.2405</v>
-      </c>
-      <c r="P30">
-        <v>-51.0664</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>92</v>
-      </c>
-      <c r="R30" t="s">
-        <v>88</v>
-      </c>
-      <c r="S30">
-        <v>140</v>
-      </c>
-      <c r="T30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="I31" t="s">
-        <v>62</v>
-      </c>
-      <c r="J31">
-        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>